<commit_message>
commit sau cuộc họp 14.10
</commit_message>
<xml_diff>
--- a/QuanLyMoiTruong.WebApp/Assets/Template/MauBaoCaoCapGiayPhepMoiTruong.xlsx
+++ b/QuanLyMoiTruong.WebApp/Assets/Template/MauBaoCaoCapGiayPhepMoiTruong.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VNPT\QuanLyThueDat\QuanLyMoiTruong\QuanLyMoiTruong.WebApp\Assets\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8514B02-3D78-4158-94EB-B36DE93D9639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601E7B88-AD0A-4D03-A4E3-A1AEE18D7EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>UBND TỈNH NGHỆ AN</t>
   </si>
@@ -52,6 +52,18 @@
   </si>
   <si>
     <t>Tên doanh nghiệp</t>
+  </si>
+  <si>
+    <t>Địa chỉ</t>
+  </si>
+  <si>
+    <t>Quy mô</t>
+  </si>
+  <si>
+    <t>Loại hình sản xuất</t>
+  </si>
+  <si>
+    <t>Tên người đại diện</t>
   </si>
 </sst>
 </file>
@@ -106,23 +118,21 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -134,29 +144,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -438,84 +453,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F6"/>
+  <dimension ref="A2:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="52.42578125" customWidth="1"/>
-    <col min="3" max="3" width="44.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="3" max="7" width="44.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:10" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:10" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="I7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="J7" s="7" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A5:J5"/>
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>